<commit_message>
excel file is changed
</commit_message>
<xml_diff>
--- a/reflection/Controller.xlsx
+++ b/reflection/Controller.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CloneCopy\morningJan2026\reflection\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F722F69A-B6D8-47F9-9A32-DD872B8F0038}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5313FC8-92D6-4FF3-B81C-ECE0D94E38EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="7236" yWindow="2448" windowWidth="9480" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -414,7 +414,7 @@
         <v>6</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
@@ -425,7 +425,7 @@
         <v>6</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>